<commit_message>
Adjusted the excel file option
</commit_message>
<xml_diff>
--- a/templates/rob_bike/DAILY MONITORING PTP, DEPO & REPO REPORT TEMPLATE.xlsx
+++ b/templates/rob_bike/DAILY MONITORING PTP, DEPO & REPO REPORT TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPM\Documents\UPDATE_FILE\VSCODE\bpi_automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPM\Documents\VSCODE\spm_automation\templates\rob_bike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C099B3E3-3E29-4A4C-B868-CA708AF35558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8281C7-0263-4ACD-A5EC-E5905BAFD2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2A8ADC3F-2E9F-4140-9B94-FC883A5D5D26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A8ADC3F-2E9F-4140-9B94-FC883A5D5D26}"/>
   </bookViews>
   <sheets>
     <sheet name="MONITORING" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB94F83-117B-432F-8D63-CC3C03370F1A}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,15 +808,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973BA036-E4CF-4A2A-9627-6C5C009CDB08}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
@@ -904,9 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE18C21A-B9E0-43B9-B7FF-D995E8EB6C28}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -995,7 +991,7 @@
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
     <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>